<commit_message>
Add WTP and Human Capital costs for Sequelae
</commit_message>
<xml_diff>
--- a/Data/WTPvalues.xlsx
+++ b/Data/WTPvalues.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angus/Documents/AustralianFoodborneIllnessCosting/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A281D645-21AE-3F40-A576-D88F0EC96FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F092DA6-CC7C-A34E-828F-909001D09457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14160" xr2:uid="{21524838-BEF9-CD4B-85A7-806F5D6A144B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
   <si>
     <t>symptom</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>GBS</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>per day</t>
+  </si>
+  <si>
+    <t>per year</t>
   </si>
 </sst>
 </file>
@@ -418,15 +427,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03CF6502-DA3C-EB48-82A9-A0039A5699CA}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,8 +445,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -447,8 +459,11 @@
       <c r="C2">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -458,8 +473,11 @@
       <c r="C3">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -469,8 +487,11 @@
       <c r="C4">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -480,8 +501,11 @@
       <c r="C5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -489,11 +513,14 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <f>964/365</f>
-        <v>2.6410958904109587</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <f>964</f>
+        <v>964</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -501,11 +528,14 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <f>344/365</f>
-        <v>0.94246575342465755</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <f>344</f>
+        <v>344</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -513,11 +543,14 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <f>1166/365</f>
-        <v>3.1945205479452055</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <f>1166</f>
+        <v>1166</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -525,11 +558,14 @@
         <v>4</v>
       </c>
       <c r="C9">
-        <f>605/365</f>
-        <v>1.6575342465753424</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <f>605</f>
+        <v>605</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -537,20 +573,56 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <f>1620/365</f>
-        <v>4.4383561643835616</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <f>1620</f>
+        <v>1620</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <f>901</f>
+        <v>901</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C11">
-        <f>1371/365</f>
-        <v>3.7561643835616438</v>
+      <c r="C12">
+        <f>1371</f>
+        <v>1371</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <f>762</f>
+        <v>762</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>